<commit_message>
usecase e2e now working.
</commit_message>
<xml_diff>
--- a/dlt-evaluation/dlts.xlsx
+++ b/dlt-evaluation/dlts.xlsx
@@ -1,32 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastianka\Git\thesis\dlt-evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9389331A-F50B-44FC-969F-F530AA2DEFD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20568801-2653-4088-90CD-5DC5B0752D9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8BEB6102-2152-4DB8-A745-B4CF60D7DDA7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8BEB6102-2152-4DB8-A745-B4CF60D7DDA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed-Overview" sheetId="10" r:id="rId1"/>
-    <sheet name="Pre-Selection" sheetId="12" r:id="rId2"/>
-    <sheet name="_financial" sheetId="1" r:id="rId3"/>
-    <sheet name="_forbes" sheetId="2" r:id="rId4"/>
-    <sheet name="_cryptomiso" sheetId="5" r:id="rId5"/>
-    <sheet name="_coincodecap" sheetId="6" r:id="rId6"/>
-    <sheet name="_blocktivity" sheetId="8" r:id="rId7"/>
-    <sheet name="_iot" sheetId="9" r:id="rId8"/>
+    <sheet name="Pre-Selection (2)" sheetId="13" r:id="rId2"/>
+    <sheet name="Pre-Selection" sheetId="12" r:id="rId3"/>
+    <sheet name="_financial" sheetId="1" r:id="rId4"/>
+    <sheet name="_forbes" sheetId="2" r:id="rId5"/>
+    <sheet name="_cryptomiso" sheetId="5" r:id="rId6"/>
+    <sheet name="_coincodecap" sheetId="6" r:id="rId7"/>
+    <sheet name="_blocktivity" sheetId="8" r:id="rId8"/>
+    <sheet name="_iot" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">_coincodecap!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">_cryptomiso!$A$2:$H$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">_financial!$A$1:$I$201</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pre-Selection'!$A$1:$G$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">_coincodecap!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">_cryptomiso!$A$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">_financial!$A$1:$I$201</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pre-Selection'!$A$1:$G$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pre-Selection (2)'!$A$1:$F$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -215,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="1498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="1498">
   <si>
     <t>BitcoinBTC</t>
   </si>
@@ -4853,7 +4857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4925,12 +4929,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -4956,6 +4982,67 @@
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4970,6 +5057,468 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Kriterien</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-36C6-4EF5-8D9C-CC176C01F4D5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-36C6-4EF5-8D9C-CC176C01F4D5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-36C6-4EF5-8D9C-CC176C01F4D5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-36C6-4EF5-8D9C-CC176C01F4D5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pre-Selection (2)'!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Business
+Relevance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Github
+Activity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Blockchain
+Activity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>IOT
+Blockchain</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pre-Selection (2)'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-36C6-4EF5-8D9C-CC176C01F4D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -5524,7 +6073,561 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr/>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="254">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6042,6 +7145,49 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D43B524C-8A26-469B-956C-19AFB72A9CB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>9</xdr:row>
@@ -6441,10 +7587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C08E5DB-7158-42FD-8EA9-23F922FCA55F}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6465,23 +7611,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>1427</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35" t="s">
         <v>1428</v>
       </c>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:14" s="11" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
@@ -7014,13 +8160,13 @@
     <mergeCell ref="J1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:I1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="(yes)">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="(yes)">
       <formula>NOT(ISERROR(SEARCH("(yes)",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7045,6 +8191,499 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF05BF0-8418-45E3-A554-CB8D25E784BD}">
+  <dimension ref="A1:R33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" style="29" customWidth="1"/>
+    <col min="4" max="4" width="10" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10" style="29" customWidth="1"/>
+    <col min="8" max="8" width="17.21875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="34" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>1471</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:18" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="38">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38">
+        <v>1</v>
+      </c>
+      <c r="D2" s="38">
+        <v>1</v>
+      </c>
+      <c r="E2" s="38">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="34" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F4" s="37">
+        <f ca="1">((IF(ISBLANK(B4),0,INDIRECT("B2")))+(IF(ISBLANK(C4),0,INDIRECT("C2")))+(IF(ISBLANK(D4),0,INDIRECT("D2")))+(IF(ISBLANK(E4),0,INDIRECT("E2"))))</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>1473</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F5" s="37">
+        <f t="shared" ref="F5:F33" ca="1" si="0">((IF(ISBLANK(B5),0,INDIRECT("B2")))+(IF(ISBLANK(C5),0,INDIRECT("C2")))+(IF(ISBLANK(D5),0,INDIRECT("D2")))+(IF(ISBLANK(E5),0,INDIRECT("E2"))))</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>1476</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F6" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>1474</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F7" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>1475</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F8" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F9" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>1495</v>
+      </c>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F10" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F11" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F12" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F13" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="R13" s="34"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1353</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F14" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R14" s="34"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F15" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F16" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F17" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F18" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>405</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F19" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F20" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F21" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F22" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F23" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F24" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F25" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F26" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F27" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F28" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F29" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F30" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F31" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F32" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F33" s="37">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F33" xr:uid="{E2AF1D08-CD17-4973-8042-20297AF0B9DA}"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="top10" dxfId="1" priority="2" rank="10"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF475A9-C7AD-4C76-883E-EA04BE9F0EFE}">
   <dimension ref="A1:K36"/>
   <sheetViews>
@@ -7138,7 +8777,7 @@
         <v>1280</v>
       </c>
       <c r="G4" s="13">
-        <f ca="1">((IF(ISBLANK(B4),0,INDIRECT("B2")))+(IF(ISBLANK(C4),0,INDIRECT("C2")))+(IF(ISBLANK(D4),0,INDIRECT("D2")))+(IF(ISBLANK(E4),0,INDIRECT("E2")))+(IF(ISBLANK(F4),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ref="G4:G36" ca="1" si="0">((IF(ISBLANK(B4),0,INDIRECT("B2")))+(IF(ISBLANK(C4),0,INDIRECT("C2")))+(IF(ISBLANK(D4),0,INDIRECT("D2")))+(IF(ISBLANK(E4),0,INDIRECT("E2")))+(IF(ISBLANK(F4),0,INDIRECT("F2"))))*100</f>
         <v>5</v>
       </c>
       <c r="I4" s="22" t="s">
@@ -7162,7 +8801,7 @@
         <v>1280</v>
       </c>
       <c r="G5" s="13">
-        <f ca="1">((IF(ISBLANK(B5),0,INDIRECT("B2")))+(IF(ISBLANK(C5),0,INDIRECT("C2")))+(IF(ISBLANK(D5),0,INDIRECT("D2")))+(IF(ISBLANK(E5),0,INDIRECT("E2")))+(IF(ISBLANK(F5),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>55.000000000000007</v>
       </c>
       <c r="I5" s="22" t="s">
@@ -7183,7 +8822,7 @@
         <v>1280</v>
       </c>
       <c r="G6" s="13">
-        <f ca="1">((IF(ISBLANK(B6),0,INDIRECT("B2")))+(IF(ISBLANK(C6),0,INDIRECT("C2")))+(IF(ISBLANK(D6),0,INDIRECT("D2")))+(IF(ISBLANK(E6),0,INDIRECT("E2")))+(IF(ISBLANK(F6),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>25</v>
       </c>
       <c r="I6" s="25" t="s">
@@ -7207,7 +8846,7 @@
         <v>1280</v>
       </c>
       <c r="G7" s="13">
-        <f ca="1">((IF(ISBLANK(B7),0,INDIRECT("B2")))+(IF(ISBLANK(C7),0,INDIRECT("C2")))+(IF(ISBLANK(D7),0,INDIRECT("D2")))+(IF(ISBLANK(E7),0,INDIRECT("E2")))+(IF(ISBLANK(F7),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>55.000000000000007</v>
       </c>
     </row>
@@ -7219,7 +8858,7 @@
         <v>1280</v>
       </c>
       <c r="G8" s="13">
-        <f ca="1">((IF(ISBLANK(B8),0,INDIRECT("B2")))+(IF(ISBLANK(C8),0,INDIRECT("C2")))+(IF(ISBLANK(D8),0,INDIRECT("D2")))+(IF(ISBLANK(E8),0,INDIRECT("E2")))+(IF(ISBLANK(F8),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7231,7 +8870,7 @@
         <v>1280</v>
       </c>
       <c r="G9" s="13">
-        <f ca="1">((IF(ISBLANK(B9),0,INDIRECT("B2")))+(IF(ISBLANK(C9),0,INDIRECT("C2")))+(IF(ISBLANK(D9),0,INDIRECT("D2")))+(IF(ISBLANK(E9),0,INDIRECT("E2")))+(IF(ISBLANK(F9),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
       <c r="I9" s="25" t="s">
@@ -7250,7 +8889,7 @@
         <v>1280</v>
       </c>
       <c r="G10" s="13">
-        <f ca="1">((IF(ISBLANK(B10),0,INDIRECT("B2")))+(IF(ISBLANK(C10),0,INDIRECT("C2")))+(IF(ISBLANK(D10),0,INDIRECT("D2")))+(IF(ISBLANK(E10),0,INDIRECT("E2")))+(IF(ISBLANK(F10),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7268,7 +8907,7 @@
         <v>1280</v>
       </c>
       <c r="G11" s="13">
-        <f ca="1">((IF(ISBLANK(B11),0,INDIRECT("B2")))+(IF(ISBLANK(C11),0,INDIRECT("C2")))+(IF(ISBLANK(D11),0,INDIRECT("D2")))+(IF(ISBLANK(E11),0,INDIRECT("E2")))+(IF(ISBLANK(F11),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
     </row>
@@ -7289,7 +8928,7 @@
         <v>1280</v>
       </c>
       <c r="G12" s="13">
-        <f ca="1">((IF(ISBLANK(B12),0,INDIRECT("B2")))+(IF(ISBLANK(C12),0,INDIRECT("C2")))+(IF(ISBLANK(D12),0,INDIRECT("D2")))+(IF(ISBLANK(E12),0,INDIRECT("E2")))+(IF(ISBLANK(F12),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>75</v>
       </c>
     </row>
@@ -7301,7 +8940,7 @@
         <v>1280</v>
       </c>
       <c r="G13" s="13">
-        <f ca="1">((IF(ISBLANK(B13),0,INDIRECT("B2")))+(IF(ISBLANK(C13),0,INDIRECT("C2")))+(IF(ISBLANK(D13),0,INDIRECT("D2")))+(IF(ISBLANK(E13),0,INDIRECT("E2")))+(IF(ISBLANK(F13),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -7313,7 +8952,7 @@
         <v>1280</v>
       </c>
       <c r="G14" s="13">
-        <f ca="1">((IF(ISBLANK(B14),0,INDIRECT("B2")))+(IF(ISBLANK(C14),0,INDIRECT("C2")))+(IF(ISBLANK(D14),0,INDIRECT("D2")))+(IF(ISBLANK(E14),0,INDIRECT("E2")))+(IF(ISBLANK(F14),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -7325,7 +8964,7 @@
         <v>1280</v>
       </c>
       <c r="G15" s="13">
-        <f ca="1">((IF(ISBLANK(B15),0,INDIRECT("B2")))+(IF(ISBLANK(C15),0,INDIRECT("C2")))+(IF(ISBLANK(D15),0,INDIRECT("D2")))+(IF(ISBLANK(E15),0,INDIRECT("E2")))+(IF(ISBLANK(F15),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7337,7 +8976,7 @@
         <v>1280</v>
       </c>
       <c r="G16" s="13">
-        <f ca="1">((IF(ISBLANK(B16),0,INDIRECT("B2")))+(IF(ISBLANK(C16),0,INDIRECT("C2")))+(IF(ISBLANK(D16),0,INDIRECT("D2")))+(IF(ISBLANK(E16),0,INDIRECT("E2")))+(IF(ISBLANK(F16),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -7352,7 +8991,7 @@
         <v>1280</v>
       </c>
       <c r="G17" s="13">
-        <f ca="1">((IF(ISBLANK(B17),0,INDIRECT("B2")))+(IF(ISBLANK(C17),0,INDIRECT("C2")))+(IF(ISBLANK(D17),0,INDIRECT("D2")))+(IF(ISBLANK(E17),0,INDIRECT("E2")))+(IF(ISBLANK(F17),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
     </row>
@@ -7364,7 +9003,7 @@
         <v>1280</v>
       </c>
       <c r="G18" s="13">
-        <f ca="1">((IF(ISBLANK(B18),0,INDIRECT("B2")))+(IF(ISBLANK(C18),0,INDIRECT("C2")))+(IF(ISBLANK(D18),0,INDIRECT("D2")))+(IF(ISBLANK(E18),0,INDIRECT("E2")))+(IF(ISBLANK(F18),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7376,7 +9015,7 @@
         <v>1280</v>
       </c>
       <c r="G19" s="13">
-        <f ca="1">((IF(ISBLANK(B19),0,INDIRECT("B2")))+(IF(ISBLANK(C19),0,INDIRECT("C2")))+(IF(ISBLANK(D19),0,INDIRECT("D2")))+(IF(ISBLANK(E19),0,INDIRECT("E2")))+(IF(ISBLANK(F19),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7388,7 +9027,7 @@
         <v>1280</v>
       </c>
       <c r="G20" s="13">
-        <f ca="1">((IF(ISBLANK(B20),0,INDIRECT("B2")))+(IF(ISBLANK(C20),0,INDIRECT("C2")))+(IF(ISBLANK(D20),0,INDIRECT("D2")))+(IF(ISBLANK(E20),0,INDIRECT("E2")))+(IF(ISBLANK(F20),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7400,7 +9039,7 @@
         <v>1280</v>
       </c>
       <c r="G21" s="13">
-        <f ca="1">((IF(ISBLANK(B21),0,INDIRECT("B2")))+(IF(ISBLANK(C21),0,INDIRECT("C2")))+(IF(ISBLANK(D21),0,INDIRECT("D2")))+(IF(ISBLANK(E21),0,INDIRECT("E2")))+(IF(ISBLANK(F21),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -7412,7 +9051,7 @@
         <v>1280</v>
       </c>
       <c r="G22" s="13">
-        <f ca="1">((IF(ISBLANK(B22),0,INDIRECT("B2")))+(IF(ISBLANK(C22),0,INDIRECT("C2")))+(IF(ISBLANK(D22),0,INDIRECT("D2")))+(IF(ISBLANK(E22),0,INDIRECT("E2")))+(IF(ISBLANK(F22),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7424,7 +9063,7 @@
         <v>1280</v>
       </c>
       <c r="G23" s="13">
-        <f ca="1">((IF(ISBLANK(B23),0,INDIRECT("B2")))+(IF(ISBLANK(C23),0,INDIRECT("C2")))+(IF(ISBLANK(D23),0,INDIRECT("D2")))+(IF(ISBLANK(E23),0,INDIRECT("E2")))+(IF(ISBLANK(F23),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7436,7 +9075,7 @@
         <v>1280</v>
       </c>
       <c r="G24" s="13">
-        <f ca="1">((IF(ISBLANK(B24),0,INDIRECT("B2")))+(IF(ISBLANK(C24),0,INDIRECT("C2")))+(IF(ISBLANK(D24),0,INDIRECT("D2")))+(IF(ISBLANK(E24),0,INDIRECT("E2")))+(IF(ISBLANK(F24),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7448,7 +9087,7 @@
         <v>1280</v>
       </c>
       <c r="G25" s="13">
-        <f ca="1">((IF(ISBLANK(B25),0,INDIRECT("B2")))+(IF(ISBLANK(C25),0,INDIRECT("C2")))+(IF(ISBLANK(D25),0,INDIRECT("D2")))+(IF(ISBLANK(E25),0,INDIRECT("E2")))+(IF(ISBLANK(F25),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -7463,7 +9102,7 @@
         <v>1280</v>
       </c>
       <c r="G26" s="13">
-        <f ca="1">((IF(ISBLANK(B26),0,INDIRECT("B2")))+(IF(ISBLANK(C26),0,INDIRECT("C2")))+(IF(ISBLANK(D26),0,INDIRECT("D2")))+(IF(ISBLANK(E26),0,INDIRECT("E2")))+(IF(ISBLANK(F26),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
     </row>
@@ -7475,7 +9114,7 @@
         <v>1280</v>
       </c>
       <c r="G27" s="13">
-        <f ca="1">((IF(ISBLANK(B27),0,INDIRECT("B2")))+(IF(ISBLANK(C27),0,INDIRECT("C2")))+(IF(ISBLANK(D27),0,INDIRECT("D2")))+(IF(ISBLANK(E27),0,INDIRECT("E2")))+(IF(ISBLANK(F27),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -7487,7 +9126,7 @@
         <v>1280</v>
       </c>
       <c r="G28" s="13">
-        <f ca="1">((IF(ISBLANK(B28),0,INDIRECT("B2")))+(IF(ISBLANK(C28),0,INDIRECT("C2")))+(IF(ISBLANK(D28),0,INDIRECT("D2")))+(IF(ISBLANK(E28),0,INDIRECT("E2")))+(IF(ISBLANK(F28),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -7499,7 +9138,7 @@
         <v>1280</v>
       </c>
       <c r="G29" s="13">
-        <f ca="1">((IF(ISBLANK(B29),0,INDIRECT("B2")))+(IF(ISBLANK(C29),0,INDIRECT("C2")))+(IF(ISBLANK(D29),0,INDIRECT("D2")))+(IF(ISBLANK(E29),0,INDIRECT("E2")))+(IF(ISBLANK(F29),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7514,7 +9153,7 @@
         <v>1280</v>
       </c>
       <c r="G30" s="13">
-        <f ca="1">((IF(ISBLANK(B30),0,INDIRECT("B2")))+(IF(ISBLANK(C30),0,INDIRECT("C2")))+(IF(ISBLANK(D30),0,INDIRECT("D2")))+(IF(ISBLANK(E30),0,INDIRECT("E2")))+(IF(ISBLANK(F30),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
     </row>
@@ -7526,7 +9165,7 @@
         <v>1280</v>
       </c>
       <c r="G31" s="13">
-        <f ca="1">((IF(ISBLANK(B31),0,INDIRECT("B2")))+(IF(ISBLANK(C31),0,INDIRECT("C2")))+(IF(ISBLANK(D31),0,INDIRECT("D2")))+(IF(ISBLANK(E31),0,INDIRECT("E2")))+(IF(ISBLANK(F31),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7538,7 +9177,7 @@
         <v>1280</v>
       </c>
       <c r="G32" s="13">
-        <f ca="1">((IF(ISBLANK(B32),0,INDIRECT("B2")))+(IF(ISBLANK(C32),0,INDIRECT("C2")))+(IF(ISBLANK(D32),0,INDIRECT("D2")))+(IF(ISBLANK(E32),0,INDIRECT("E2")))+(IF(ISBLANK(F32),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7550,7 +9189,7 @@
         <v>1280</v>
       </c>
       <c r="G33" s="13">
-        <f ca="1">((IF(ISBLANK(B33),0,INDIRECT("B2")))+(IF(ISBLANK(C33),0,INDIRECT("C2")))+(IF(ISBLANK(D33),0,INDIRECT("D2")))+(IF(ISBLANK(E33),0,INDIRECT("E2")))+(IF(ISBLANK(F33),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -7565,7 +9204,7 @@
         <v>1280</v>
       </c>
       <c r="G34" s="13">
-        <f ca="1">((IF(ISBLANK(B34),0,INDIRECT("B2")))+(IF(ISBLANK(C34),0,INDIRECT("C2")))+(IF(ISBLANK(D34),0,INDIRECT("D2")))+(IF(ISBLANK(E34),0,INDIRECT("E2")))+(IF(ISBLANK(F34),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
     </row>
@@ -7581,7 +9220,7 @@
       <c r="E35" s="20"/>
       <c r="F35" s="21"/>
       <c r="G35" s="20">
-        <f ca="1">((IF(ISBLANK(B35),0,INDIRECT("B2")))+(IF(ISBLANK(C35),0,INDIRECT("C2")))+(IF(ISBLANK(D35),0,INDIRECT("D2")))+(IF(ISBLANK(E35),0,INDIRECT("E2")))+(IF(ISBLANK(F35),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7597,7 +9236,7 @@
       <c r="E36" s="20"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20">
-        <f ca="1">((IF(ISBLANK(B36),0,INDIRECT("B2")))+(IF(ISBLANK(C36),0,INDIRECT("C2")))+(IF(ISBLANK(D36),0,INDIRECT("D2")))+(IF(ISBLANK(E36),0,INDIRECT("E2")))+(IF(ISBLANK(F36),0,INDIRECT("F2"))))*100</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -7612,7 +9251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7518A5F-563F-492B-9A43-DEB9D821B7F3}">
   <dimension ref="A1:J198"/>
   <sheetViews>
@@ -12041,7 +13680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D351F5-B84F-4452-A157-73972A78B156}">
   <dimension ref="A1:AD25"/>
   <sheetViews>
@@ -12568,7 +14207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18B65BC-6CA1-4A96-A322-22F3276505C3}">
   <dimension ref="A1:J68"/>
   <sheetViews>
@@ -12583,16 +14222,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="36" t="s">
         <v>1169</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36" t="s">
         <v>1170</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -14517,7 +16156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2104961-C87C-4EB7-BFEC-01AA1EE9FA54}">
   <dimension ref="A1:K99"/>
   <sheetViews>
@@ -16136,7 +17775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABA0B23-D0B6-46C0-9964-5E9F2F29E19B}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -16478,7 +18117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84581B7-ECA8-43C6-8ED4-4BA18810068C}">
   <dimension ref="A1:J11"/>
   <sheetViews>

</xml_diff>